<commit_message>
New links and commands
</commit_message>
<xml_diff>
--- a/Links MQTT.xlsx
+++ b/Links MQTT.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
@@ -249,6 +249,69 @@
   </si>
   <si>
     <t xml:space="preserve">https://communities.intel.com/docs/DOC-23764</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commandos Ethernet/Network (Linux)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://developer.toradex.com/knowledge-base/ethernet-network-(linux)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installing and Running applications on the Galileo Board Gen 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://docs.oracle.com/javame/8.3/get-started-galileo/installing-and-running-applications-intel-galileo-gen2-board.htm#MEEGG-GUID-F8F98050-3BE7-4E17-BFE5-72CCE9C4FBD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuración más completa Mosquitto Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://lukse.lt/uzrasai/2015-02-internet-of-things-messaging-mqtt-1-installing-mosquitto-server/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMANDOS LINUX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://linuxcommand.org/man_pages/ls1.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mosquito Guide (Broker,_sub,…..)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mosquitto.org/documentation/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIMULADORES MODBUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://docklight.de/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.plcsimulator.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial de Modbus for Galileo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.cooking-hacks.com/documentation/tutorials/modbus-module-shield-tutorial-for-arduino-raspberry-pi-intel-galileo/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foro sobre Modbus y su implementación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://stackoverflow.com/questions/tagged/modbus?page=1&amp;sort=newest&amp;pagesize=15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">microcontroladores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.freertos.org/a00090.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nModbus (Otra libreria)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.mesta-automation.com/modbus-with-c-sharp-libraries-examples/</t>
   </si>
 </sst>
 </file>
@@ -384,19 +447,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="60.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="150.918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="96.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="89.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="59.3979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="120.005102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="95.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="88.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,7 +482,7 @@
       <c r="C2" s="0"/>
       <c r="D2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -641,6 +704,7 @@
       <c r="B25" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -649,6 +713,7 @@
       <c r="B26" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
@@ -657,6 +722,7 @@
       <c r="B27" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
@@ -665,6 +731,7 @@
       <c r="B28" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="C28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -673,6 +740,7 @@
       <c r="B29" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -681,6 +749,7 @@
       <c r="B30" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
@@ -689,6 +758,7 @@
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
@@ -697,6 +767,7 @@
       <c r="B32" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="C32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -705,6 +776,7 @@
       <c r="B33" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="C33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -712,6 +784,95 @@
       </c>
       <c r="B34" s="1" t="s">
         <v>72</v>
+      </c>
+      <c r="C34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -746,7 +907,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -772,7 +933,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>